<commit_message>
Build the streamlite login functionality using email
</commit_message>
<xml_diff>
--- a/data_transformations/data/final/paragon_data_full.xlsx
+++ b/data_transformations/data/final/paragon_data_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P209"/>
+  <dimension ref="A1:P224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,7 +561,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pasta Miso As Sty 200g</t>
+          <t>pasta miso as sty</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -617,7 +617,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>JOG SKYR MIX 150G</t>
+          <t>jog skyr mix</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -673,7 +673,7 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Miesz Chińska 450g</t>
+          <t>miesz chinska</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Fasola Żół Ziel 450g</t>
+          <t>fasola zol ziel</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -793,7 +793,7 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Wiśnie Bez Pestek 450g</t>
+          <t>wisnie bez pestek</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -849,7 +849,7 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Mięs Miel Woł 400g</t>
+          <t>mies miel wol</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -905,7 +905,7 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Kieł śląs/biał 270g</t>
+          <t>kiel slasbial</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -961,7 +961,7 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>MINI SNAC PLEŚN 100g</t>
+          <t>mini snac plesn</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -1017,7 +1017,7 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Piwo Per 0 0,5l B BZW</t>
+          <t>piwo per 0  b bzw</t>
         </is>
       </c>
       <c r="M10" t="n">
@@ -1073,7 +1073,7 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Mmilc Prot Zero Cze 400g</t>
+          <t>mmilc prot zero cze</t>
         </is>
       </c>
       <c r="M11" t="n">
@@ -1129,7 +1129,7 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Mięta Kolendra XLVF</t>
+          <t>mieta kolendra xlvf</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pist Praż Sol Top 200g</t>
+          <t>pist praz sol top</t>
         </is>
       </c>
       <c r="M13" t="n">
@@ -1243,7 +1243,7 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Woda Gaz Muszy 1,5l</t>
+          <t>woda gaz muszy</t>
         </is>
       </c>
       <c r="M14" t="n">
@@ -1299,7 +1299,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Serek Prot. Malina 200g</t>
+          <t>serek prot malina</t>
         </is>
       </c>
       <c r="M15" t="n">
@@ -1355,7 +1355,7 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Piwo Per 0 0,5l B BZW</t>
+          <t>piwo per 0  b bzw</t>
         </is>
       </c>
       <c r="M16" t="n">
@@ -1411,7 +1411,7 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Nerko Migdał Top 150g</t>
+          <t>nerko migdal top</t>
         </is>
       </c>
       <c r="M17" t="n">
@@ -1467,7 +1467,7 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Kieł śląs/biał 270g</t>
+          <t>kiel slasbial</t>
         </is>
       </c>
       <c r="M18" t="n">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pierogi Ruskie 800g</t>
+          <t>pierogi ruskie</t>
         </is>
       </c>
       <c r="M19" t="n">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Fasola Żół Ziel 450g</t>
+          <t>fasola zol ziel</t>
         </is>
       </c>
       <c r="M20" t="n">
@@ -1651,7 +1651,7 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Kiełbasa Chorizo 280g</t>
+          <t>kielbasa chorizo</t>
         </is>
       </c>
       <c r="M21" t="n">
@@ -1707,7 +1707,7 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>BWę/ Par Morlin 150 g</t>
+          <t>bwe par morlin</t>
         </is>
       </c>
       <c r="M22" t="n">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O22" t="n">
@@ -1763,7 +1763,7 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Ser Edamski 250g</t>
+          <t>ser edamski</t>
         </is>
       </c>
       <c r="M23" t="n">
@@ -1819,7 +1819,7 @@
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Serek z palusz 35g</t>
+          <t>serek z palusz</t>
         </is>
       </c>
       <c r="M24" t="n">
@@ -1875,7 +1875,7 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Mięta Kolendra XLVF</t>
+          <t>mieta kolendra xlvf</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -1925,7 +1925,7 @@
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Limonka szt</t>
+          <t>limonka szt</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -1975,7 +1975,7 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M27" t="n">
@@ -2031,7 +2031,7 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Chipsy Top Solone 150g</t>
+          <t>chipsy top solone</t>
         </is>
       </c>
       <c r="M28" t="n">
@@ -2087,7 +2087,7 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Mmilc Prot Zero Cze 400g</t>
+          <t>mmilc prot zero cze</t>
         </is>
       </c>
       <c r="M29" t="n">
@@ -2143,7 +2143,7 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Lod Mag Almond 110ml</t>
+          <t>lod mag almond</t>
         </is>
       </c>
       <c r="M30" t="n">
@@ -2199,7 +2199,7 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Wafle Chrup Asy 90g</t>
+          <t>wafle chrup asy</t>
         </is>
       </c>
       <c r="M31" t="n">
@@ -2255,7 +2255,7 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Cebula Żółta Luz</t>
+          <t>cebula zolta luz</t>
         </is>
       </c>
       <c r="M32" t="inlineStr"/>
@@ -2305,7 +2305,7 @@
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Młyn Sól Mor Kami 90 g</t>
+          <t>mlyn sol mor kami</t>
         </is>
       </c>
       <c r="M33" t="n">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O33" t="n">
@@ -2361,7 +2361,7 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Mł Piepr Cz Kamis 42 g</t>
+          <t>ml piepr cz kamis</t>
         </is>
       </c>
       <c r="M34" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O34" t="n">
@@ -2417,7 +2417,7 @@
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Piwo Per 0 0,5l B BZW</t>
+          <t>piwo per 0  b bzw</t>
         </is>
       </c>
       <c r="M35" t="n">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Krem Neutral Sma 70g Mix</t>
+          <t>krem neutral sma  mix</t>
         </is>
       </c>
       <c r="M36" t="n">
@@ -2537,7 +2537,7 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Wor Ecofa Zos 120lx 10</t>
+          <t>wor ecofa zos 120lx 10</t>
         </is>
       </c>
       <c r="M37" t="n">
@@ -2593,7 +2593,7 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Ręk Nitryl M 50szt</t>
+          <t>rek nitryl m</t>
         </is>
       </c>
       <c r="M38" t="n">
@@ -2649,7 +2649,7 @@
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Bocz. Węd/ Par 100g.</t>
+          <t xml:space="preserve">bocz wed par </t>
         </is>
       </c>
       <c r="M39" t="n">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Szyn z Wędzarni KW 200g</t>
+          <t>szyn z wedzarni kw</t>
         </is>
       </c>
       <c r="M40" t="n">
@@ -2769,7 +2769,7 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Przyprawa Maggi 200g</t>
+          <t>przyprawa maggi</t>
         </is>
       </c>
       <c r="M41" t="n">
@@ -2825,7 +2825,7 @@
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Sos Sałatk Włos Knorr 8g</t>
+          <t>sos salatk wlos knorr</t>
         </is>
       </c>
       <c r="M42" t="n">
@@ -2889,7 +2889,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Masło Ekst Łowic 200g</t>
+          <t>maslo ekst lowic</t>
         </is>
       </c>
       <c r="M43" t="n">
@@ -2945,7 +2945,7 @@
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Ser Rycerski Świ 135g</t>
+          <t>ser rycerski swi</t>
         </is>
       </c>
       <c r="M44" t="n">
@@ -3009,7 +3009,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Twarnat 150g 200g</t>
+          <t>twarnat  200g</t>
         </is>
       </c>
       <c r="M45" t="n">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Jog nat Activ 165g</t>
+          <t>jog nat activ</t>
         </is>
       </c>
       <c r="M46" t="n">
@@ -3129,7 +3129,7 @@
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Twaróg Półtł 250g</t>
+          <t>twarog poltl</t>
         </is>
       </c>
       <c r="M47" t="n">
@@ -3185,7 +3185,7 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Worki Śmi JN 60l 20szt</t>
+          <t>worki smi jn  20szt</t>
         </is>
       </c>
       <c r="M48" t="n">
@@ -3241,7 +3241,7 @@
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Drożdż ZSerem 130g</t>
+          <t>drozdz zserem</t>
         </is>
       </c>
       <c r="M49" t="n">
@@ -3297,7 +3297,7 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Paluch Zoliwk 80g</t>
+          <t>paluch zoliwk</t>
         </is>
       </c>
       <c r="M50" t="n">
@@ -3353,7 +3353,7 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Bułka Codzienna 100g</t>
+          <t>bulka codzienna</t>
         </is>
       </c>
       <c r="M51" t="n">
@@ -3409,7 +3409,7 @@
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Jaja W Wyb L 10szt</t>
+          <t>jaja w wyb l</t>
         </is>
       </c>
       <c r="M52" t="n">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pierogi Ruskie 800g</t>
+          <t>pierogi ruskie</t>
         </is>
       </c>
       <c r="M53" t="n">
@@ -3529,7 +3529,7 @@
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Fasol Heinz 415g</t>
+          <t>fasol heinz</t>
         </is>
       </c>
       <c r="M54" t="n">
@@ -3585,7 +3585,7 @@
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Ser Goud Wió Świa 300g</t>
+          <t>ser goud wio swia</t>
         </is>
       </c>
       <c r="M55" t="n">
@@ -3641,7 +3641,7 @@
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Passata Gust Bel 690g</t>
+          <t>passata gust bel</t>
         </is>
       </c>
       <c r="M56" t="n">
@@ -3697,7 +3697,7 @@
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Piwo Per 0 0,5l B BZW</t>
+          <t>piwo per 0  b bzw</t>
         </is>
       </c>
       <c r="M57" t="n">
@@ -3753,7 +3753,7 @@
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Serek W Wysokobia 200g</t>
+          <t>serek w wysokobia</t>
         </is>
       </c>
       <c r="M58" t="n">
@@ -3809,7 +3809,7 @@
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Owocowy Mix MK 450g</t>
+          <t>owocowy mix mk</t>
         </is>
       </c>
       <c r="M59" t="n">
@@ -3865,7 +3865,7 @@
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr">
         <is>
-          <t>BWę/ Par Morlin 150 g</t>
+          <t>bwe par morlin</t>
         </is>
       </c>
       <c r="M60" t="n">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O60" t="n">
@@ -3921,7 +3921,7 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Cebula Żółta Luz</t>
+          <t>cebula zolta luz</t>
         </is>
       </c>
       <c r="M61" t="inlineStr"/>
@@ -3971,7 +3971,7 @@
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pietruszka Don XLVF</t>
+          <t>pietruszka don xlvf</t>
         </is>
       </c>
       <c r="M62" t="inlineStr"/>
@@ -4021,7 +4021,7 @@
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Mięta Kolendra XLVF</t>
+          <t>mieta kolendra xlvf</t>
         </is>
       </c>
       <c r="M63" t="inlineStr"/>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Fasola Żół Ziel 450g</t>
+          <t>fasola zol ziel</t>
         </is>
       </c>
       <c r="M64" t="n">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Mięs Miel Woł 400g</t>
+          <t>mies miel wol</t>
         </is>
       </c>
       <c r="M65" t="n">
@@ -4199,7 +4199,7 @@
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M66" t="n">
@@ -4255,7 +4255,7 @@
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Ręcz Mega Sweep 100</t>
+          <t>recz mega sweep 100</t>
         </is>
       </c>
       <c r="M67" t="inlineStr"/>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Serek Prot Wanilia 200g</t>
+          <t>serek prot wanilia</t>
         </is>
       </c>
       <c r="M68" t="n">
@@ -4377,7 +4377,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Deser Monte 150g</t>
+          <t>deser monte</t>
         </is>
       </c>
       <c r="M69" t="n">
@@ -4433,7 +4433,7 @@
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Szczypiorek Natka</t>
+          <t>szczypiorek natka</t>
         </is>
       </c>
       <c r="M70" t="inlineStr"/>
@@ -4483,7 +4483,7 @@
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pieczar 200g opak</t>
+          <t>pieczar  opak</t>
         </is>
       </c>
       <c r="M71" t="n">
@@ -4539,7 +4539,7 @@
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Imbir luz</t>
+          <t>imbir luz</t>
         </is>
       </c>
       <c r="M72" t="inlineStr"/>
@@ -4589,7 +4589,7 @@
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Banan kiść bio</t>
+          <t>banan kisc bio</t>
         </is>
       </c>
       <c r="M73" t="inlineStr"/>
@@ -4639,7 +4639,7 @@
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr">
         <is>
-          <t>ŚM PRIM 30 ZOT 200G</t>
+          <t>sm prim 30 zot</t>
         </is>
       </c>
       <c r="M74" t="n">
@@ -4695,7 +4695,7 @@
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Kefir Krasnyst 420g</t>
+          <t>kefir krasnyst</t>
         </is>
       </c>
       <c r="M75" t="n">
@@ -4751,7 +4751,7 @@
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Jabł Polskie Gala Luz</t>
+          <t>jabl polskie gala luz</t>
         </is>
       </c>
       <c r="M76" t="inlineStr"/>
@@ -4801,7 +4801,7 @@
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Limonka szt</t>
+          <t>limonka szt</t>
         </is>
       </c>
       <c r="M77" t="inlineStr"/>
@@ -4851,7 +4851,7 @@
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Crois Nad Orz Kak 85g</t>
+          <t>crois nad orz kak</t>
         </is>
       </c>
       <c r="M78" t="n">
@@ -4915,7 +4915,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Kieł śląs/biał 270g</t>
+          <t>kiel slasbial</t>
         </is>
       </c>
       <c r="M79" t="n">
@@ -4971,7 +4971,7 @@
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Lod Marl Almond 120ml</t>
+          <t>lod marl almond</t>
         </is>
       </c>
       <c r="M80" t="n">
@@ -5027,7 +5027,7 @@
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Żel Ener Go Activ 100g</t>
+          <t>zel ener go activ</t>
         </is>
       </c>
       <c r="M81" t="n">
@@ -5083,7 +5083,7 @@
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M82" t="n">
@@ -5139,7 +5139,7 @@
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Jaja Wol Wyb M 20szt</t>
+          <t>jaja wol wyb m</t>
         </is>
       </c>
       <c r="M83" t="n">
@@ -5195,7 +5195,7 @@
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Miesz Chińska 450g</t>
+          <t>miesz chinska</t>
         </is>
       </c>
       <c r="M84" t="n">
@@ -5251,7 +5251,7 @@
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pom Mal Podłużny 500g</t>
+          <t>pom mal podluzny</t>
         </is>
       </c>
       <c r="M85" t="n">
@@ -5307,7 +5307,7 @@
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Nap. Prot Go Acti 250g</t>
+          <t>nap prot go acti</t>
         </is>
       </c>
       <c r="M86" t="n">
@@ -5363,7 +5363,7 @@
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Jog Pit Sky Piąt 330ml</t>
+          <t>jog pit sky piat</t>
         </is>
       </c>
       <c r="M87" t="n">
@@ -5419,7 +5419,7 @@
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Rukola Myta VF 100g</t>
+          <t>rukola myta vf</t>
         </is>
       </c>
       <c r="M88" t="n">
@@ -5475,7 +5475,7 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Serek Prot Wanilia 200g</t>
+          <t>serek prot wanilia</t>
         </is>
       </c>
       <c r="M89" t="n">
@@ -5531,7 +5531,7 @@
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Serek Prot. Malina 200g</t>
+          <t>serek prot malina</t>
         </is>
       </c>
       <c r="M90" t="n">
@@ -5587,7 +5587,7 @@
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Serek Prot Brz- Mar 200g</t>
+          <t>serek prot brz mar</t>
         </is>
       </c>
       <c r="M91" t="n">
@@ -5643,7 +5643,7 @@
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M92" t="n">
@@ -5699,7 +5699,7 @@
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr">
         <is>
-          <t>Mięta Kolendra XLVF</t>
+          <t>mieta kolendra xlvf</t>
         </is>
       </c>
       <c r="M93" t="inlineStr"/>
@@ -5749,7 +5749,7 @@
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr">
         <is>
-          <t>Papr Jal A Flav 110g</t>
+          <t>papr jal a flav</t>
         </is>
       </c>
       <c r="M94" t="n">
@@ -5805,7 +5805,7 @@
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr">
         <is>
-          <t>Serek Prot Wanilia 200g</t>
+          <t>serek prot wanilia</t>
         </is>
       </c>
       <c r="M95" t="n">
@@ -5861,7 +5861,7 @@
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr">
         <is>
-          <t>Piwo Per 0 0,5l B BZW</t>
+          <t>piwo per 0  b bzw</t>
         </is>
       </c>
       <c r="M96" t="n">
@@ -5917,7 +5917,7 @@
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr">
         <is>
-          <t>Triple Crem Deli Ga 180g</t>
+          <t>triple crem deli ga</t>
         </is>
       </c>
       <c r="M97" t="n">
@@ -5973,7 +5973,7 @@
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr">
         <is>
-          <t>Sal z oliwkami i baz</t>
+          <t>sal z oliwkami i baz</t>
         </is>
       </c>
       <c r="M98" t="inlineStr"/>
@@ -6023,7 +6023,7 @@
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr">
         <is>
-          <t>Nap Gaz Dr Pepp Reg 0,33l</t>
+          <t>nap gaz dr pepp reg</t>
         </is>
       </c>
       <c r="M99" t="n">
@@ -6079,7 +6079,7 @@
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr">
         <is>
-          <t>Nap Dr Pepper Cher 0,33l</t>
+          <t>nap dr pepper cher</t>
         </is>
       </c>
       <c r="M100" t="n">
@@ -6135,7 +6135,7 @@
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr">
         <is>
-          <t>BWę/ Par Morlin 150 g</t>
+          <t>bwe par morlin</t>
         </is>
       </c>
       <c r="M101" t="n">
@@ -6143,7 +6143,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O101" t="n">
@@ -6199,7 +6199,7 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>Pomarańcze Des Luz</t>
+          <t>pomarancze des luz</t>
         </is>
       </c>
       <c r="M102" t="inlineStr"/>
@@ -6249,7 +6249,7 @@
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr">
         <is>
-          <t>Ciastk Nadz Bud 35g</t>
+          <t>ciastk nadz bud</t>
         </is>
       </c>
       <c r="M103" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>Praliny Lind 200g</t>
+          <t>praliny lind</t>
         </is>
       </c>
       <c r="M104" t="n">
@@ -6377,7 +6377,7 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>Paró Szyn Nat Tarcz 200g</t>
+          <t>paro szyn nat tarcz</t>
         </is>
       </c>
       <c r="M105" t="n">
@@ -6433,7 +6433,7 @@
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr">
         <is>
-          <t>Bocz. Węd/ Par 100g.</t>
+          <t xml:space="preserve">bocz wed par </t>
         </is>
       </c>
       <c r="M106" t="n">
@@ -6489,7 +6489,7 @@
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr">
         <is>
-          <t>Pomid Paski 270 150g</t>
+          <t>pomid paski 270</t>
         </is>
       </c>
       <c r="M107" t="n">
@@ -6545,7 +6545,7 @@
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr">
         <is>
-          <t>Cam Natur Delik 120g</t>
+          <t>cam natur delik</t>
         </is>
       </c>
       <c r="M108" t="n">
@@ -6601,7 +6601,7 @@
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr">
         <is>
-          <t>Ogór Kana Na Spi 670/360</t>
+          <t>ogor kana na spi 670360</t>
         </is>
       </c>
       <c r="M109" t="inlineStr"/>
@@ -6651,7 +6651,7 @@
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr">
         <is>
-          <t>Twaróg Półtł 250g</t>
+          <t>twarog poltl</t>
         </is>
       </c>
       <c r="M110" t="n">
@@ -6707,7 +6707,7 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr">
         <is>
-          <t>Twarnat 150g 200g</t>
+          <t>twarnat  200g</t>
         </is>
       </c>
       <c r="M111" t="n">
@@ -6763,7 +6763,7 @@
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr">
         <is>
-          <t>Śmiet Pi 18 200g</t>
+          <t>smiet pi 18</t>
         </is>
       </c>
       <c r="M112" t="n">
@@ -6827,7 +6827,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>Sere. Alme. Mix 150g</t>
+          <t>sere alme mix</t>
         </is>
       </c>
       <c r="M113" t="n">
@@ -6883,7 +6883,7 @@
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr">
         <is>
-          <t>Mozzarella Light 125g</t>
+          <t>mozzarella light</t>
         </is>
       </c>
       <c r="M114" t="n">
@@ -6947,7 +6947,7 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>Pom Paprycz Luz</t>
+          <t>pom paprycz luz</t>
         </is>
       </c>
       <c r="M115" t="inlineStr"/>
@@ -6997,7 +6997,7 @@
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr">
         <is>
-          <t>Pomid gał luz</t>
+          <t>pomid gal luz</t>
         </is>
       </c>
       <c r="M116" t="inlineStr"/>
@@ -7047,7 +7047,7 @@
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr">
         <is>
-          <t>Bułka Poranna 65g</t>
+          <t>bulka poranna</t>
         </is>
       </c>
       <c r="M117" t="n">
@@ -7103,7 +7103,7 @@
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr">
         <is>
-          <t>Drożdż ZSerem 130g</t>
+          <t>drozdz zserem</t>
         </is>
       </c>
       <c r="M118" t="n">
@@ -7159,7 +7159,7 @@
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr">
         <is>
-          <t>Piwo Per 0 0,5l B BZW</t>
+          <t>piwo per 0  b bzw</t>
         </is>
       </c>
       <c r="M119" t="n">
@@ -7215,7 +7215,7 @@
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr">
         <is>
-          <t>Jaja Go Bio 9szt</t>
+          <t>jaja go bio</t>
         </is>
       </c>
       <c r="M120" t="n">
@@ -7271,7 +7271,7 @@
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr">
         <is>
-          <t>Passata Gust Bel 690g</t>
+          <t>passata gust bel</t>
         </is>
       </c>
       <c r="M121" t="n">
@@ -7327,7 +7327,7 @@
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr">
         <is>
-          <t>Worki na śmieci 60L</t>
+          <t>worki na smieci</t>
         </is>
       </c>
       <c r="M122" t="n">
@@ -7383,7 +7383,7 @@
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr">
         <is>
-          <t>Fasol Heinz 415g</t>
+          <t>fasol heinz</t>
         </is>
       </c>
       <c r="M123" t="n">
@@ -7439,7 +7439,7 @@
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr">
         <is>
-          <t>Nap Dr Peppe Canad 0,33l</t>
+          <t>nap dr peppe canad</t>
         </is>
       </c>
       <c r="M124" t="n">
@@ -7495,7 +7495,7 @@
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr">
         <is>
-          <t>Kieł śląs/biał 270g</t>
+          <t>kiel slasbial</t>
         </is>
       </c>
       <c r="M125" t="n">
@@ -7551,7 +7551,7 @@
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr">
         <is>
-          <t>Mięs Miel Woł 400g</t>
+          <t>mies miel wol</t>
         </is>
       </c>
       <c r="M126" t="n">
@@ -7607,7 +7607,7 @@
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr">
         <is>
-          <t>Chusr Mr Mag Kuch 50szt</t>
+          <t>chusr mr mag kuch</t>
         </is>
       </c>
       <c r="M127" t="n">
@@ -7663,7 +7663,7 @@
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr">
         <is>
-          <t>Chust Mr Mag Łaz 60szt</t>
+          <t>chust mr mag laz</t>
         </is>
       </c>
       <c r="M128" t="n">
@@ -7719,7 +7719,7 @@
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr">
         <is>
-          <t>Pierogi Ruskie 800g</t>
+          <t>pierogi ruskie</t>
         </is>
       </c>
       <c r="M129" t="n">
@@ -7775,7 +7775,7 @@
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr">
         <is>
-          <t>Cebula 1kg opak</t>
+          <t>cebula  opak</t>
         </is>
       </c>
       <c r="M130" t="n">
@@ -7831,7 +7831,7 @@
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr">
         <is>
-          <t>Banan Premium Luz</t>
+          <t>banan premium luz</t>
         </is>
       </c>
       <c r="M131" t="inlineStr"/>
@@ -7881,7 +7881,7 @@
       <c r="K132" t="inlineStr"/>
       <c r="L132" t="inlineStr">
         <is>
-          <t>Bagietka Czos 165g</t>
+          <t>bagietka czos</t>
         </is>
       </c>
       <c r="M132" t="n">
@@ -7937,7 +7937,7 @@
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr">
         <is>
-          <t>Crois Nad Orz Kak 85g</t>
+          <t>crois nad orz kak</t>
         </is>
       </c>
       <c r="M133" t="n">
@@ -7993,7 +7993,7 @@
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M134" t="n">
@@ -8049,7 +8049,7 @@
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr">
         <is>
-          <t>Jaja Go Bio 9szt</t>
+          <t>jaja go bio</t>
         </is>
       </c>
       <c r="M135" t="n">
@@ -8105,7 +8105,7 @@
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr">
         <is>
-          <t>Pomidor Kokt Gał 400g</t>
+          <t>pomidor kokt gal</t>
         </is>
       </c>
       <c r="M136" t="n">
@@ -8161,7 +8161,7 @@
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr">
         <is>
-          <t>Ruk Bio Go Bio 80g</t>
+          <t>ruk bio go bio</t>
         </is>
       </c>
       <c r="M137" t="n">
@@ -8217,7 +8217,7 @@
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr">
         <is>
-          <t>Olej Kokos Vit 500ml</t>
+          <t>olej kokos vit</t>
         </is>
       </c>
       <c r="M138" t="n">
@@ -8273,7 +8273,7 @@
       <c r="K139" t="inlineStr"/>
       <c r="L139" t="inlineStr">
         <is>
-          <t>Bagietka Czos 165g</t>
+          <t>bagietka czos</t>
         </is>
       </c>
       <c r="M139" t="n">
@@ -8329,7 +8329,7 @@
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M140" t="n">
@@ -8385,7 +8385,7 @@
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr">
         <is>
-          <t>Pieczarka 250g mini</t>
+          <t>pieczarka  mini</t>
         </is>
       </c>
       <c r="M141" t="n">
@@ -8441,7 +8441,7 @@
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr">
         <is>
-          <t>Pietruszka Don XLVF</t>
+          <t>pietruszka don xlvf</t>
         </is>
       </c>
       <c r="M142" t="inlineStr"/>
@@ -8491,7 +8491,7 @@
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr">
         <is>
-          <t>Oliw Terr Gus Be 500ml</t>
+          <t>oliw terr gus be</t>
         </is>
       </c>
       <c r="M143" t="n">
@@ -8547,7 +8547,7 @@
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr">
         <is>
-          <t>Torba T-SHIRT</t>
+          <t>torba tshirt</t>
         </is>
       </c>
       <c r="M144" t="inlineStr"/>
@@ -8597,7 +8597,7 @@
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr">
         <is>
-          <t>Trawa pampasow 2</t>
+          <t>trawa pampasow 2</t>
         </is>
       </c>
       <c r="M145" t="inlineStr"/>
@@ -8647,7 +8647,7 @@
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr">
         <is>
-          <t>Jog ZNiespo 75g</t>
+          <t>jog zniespo</t>
         </is>
       </c>
       <c r="M146" t="n">
@@ -8703,7 +8703,7 @@
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr">
         <is>
-          <t>JOG SKYR MIX 150G</t>
+          <t>jog skyr mix</t>
         </is>
       </c>
       <c r="M147" t="n">
@@ -8759,7 +8759,7 @@
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr">
         <is>
-          <t>JOG SKYR MIX 150G</t>
+          <t>jog skyr mix</t>
         </is>
       </c>
       <c r="M148" t="n">
@@ -8815,7 +8815,7 @@
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr">
         <is>
-          <t>JOG SKYR MIX 150G</t>
+          <t>jog skyr mix</t>
         </is>
       </c>
       <c r="M149" t="n">
@@ -8879,7 +8879,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>Mąka T 650 Plon Nat 1kg</t>
+          <t>maka t 650 plon nat</t>
         </is>
       </c>
       <c r="M150" t="n">
@@ -8935,7 +8935,7 @@
       <c r="K151" t="inlineStr"/>
       <c r="L151" t="inlineStr">
         <is>
-          <t>Nap Gaz Coca Cola 2x 2L</t>
+          <t>nap gaz coca cola 2x</t>
         </is>
       </c>
       <c r="M151" t="n">
@@ -8991,7 +8991,7 @@
       <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr">
         <is>
-          <t>Płatki Be Beauty 60</t>
+          <t>platki be beauty 60</t>
         </is>
       </c>
       <c r="M152" t="inlineStr"/>
@@ -9041,7 +9041,7 @@
       <c r="K153" t="inlineStr"/>
       <c r="L153" t="inlineStr">
         <is>
-          <t>Kan Mleczna 4x 28g</t>
+          <t>kan mleczna 4x</t>
         </is>
       </c>
       <c r="M153" t="n">
@@ -9097,7 +9097,7 @@
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr">
         <is>
-          <t>Gąbka kąpielowa</t>
+          <t>gabka kapielowa</t>
         </is>
       </c>
       <c r="M154" t="inlineStr"/>
@@ -9147,7 +9147,7 @@
       <c r="K155" t="inlineStr"/>
       <c r="L155" t="inlineStr">
         <is>
-          <t>Jog Pit Sky Piąt 330ml</t>
+          <t>jog pit sky piat</t>
         </is>
       </c>
       <c r="M155" t="n">
@@ -9203,7 +9203,7 @@
       <c r="K156" t="inlineStr"/>
       <c r="L156" t="inlineStr">
         <is>
-          <t>Mleko UHT 3,2 1l</t>
+          <t>mleko uht 32</t>
         </is>
       </c>
       <c r="M156" t="n">
@@ -9259,7 +9259,7 @@
       <c r="K157" t="inlineStr"/>
       <c r="L157" t="inlineStr">
         <is>
-          <t>Sok Nektar Hortex 3x 1l</t>
+          <t>sok nektar hortex 3x</t>
         </is>
       </c>
       <c r="M157" t="n">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>Mąka T 450 Plon Nat 1kg</t>
+          <t>maka t 450 plon nat</t>
         </is>
       </c>
       <c r="M158" t="n">
@@ -9379,7 +9379,7 @@
       <c r="K159" t="inlineStr"/>
       <c r="L159" t="inlineStr">
         <is>
-          <t>Bułka Codzienna 100g</t>
+          <t>bulka codzienna</t>
         </is>
       </c>
       <c r="M159" t="n">
@@ -9435,7 +9435,7 @@
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr">
         <is>
-          <t>Chleb 500 g</t>
+          <t>chleb</t>
         </is>
       </c>
       <c r="M160" t="n">
@@ -9443,7 +9443,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O160" t="n">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>Paszte Mix Drop 160 g</t>
+          <t>paszte mix drop</t>
         </is>
       </c>
       <c r="M161" t="n">
@@ -9507,7 +9507,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O161" t="n">
@@ -9555,7 +9555,7 @@
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr">
         <is>
-          <t>Gulasz Angielski 300g</t>
+          <t>gulasz angielski</t>
         </is>
       </c>
       <c r="M162" t="n">
@@ -9611,7 +9611,7 @@
       <c r="K163" t="inlineStr"/>
       <c r="L163" t="inlineStr">
         <is>
-          <t>Czeko Gorzka Konc 20g</t>
+          <t>czeko gorzka konc</t>
         </is>
       </c>
       <c r="M163" t="n">
@@ -9667,7 +9667,7 @@
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr">
         <is>
-          <t>Czeko Gorzka Regen 20g</t>
+          <t>czeko gorzka regen</t>
         </is>
       </c>
       <c r="M164" t="n">
@@ -9723,7 +9723,7 @@
       <c r="K165" t="inlineStr"/>
       <c r="L165" t="inlineStr">
         <is>
-          <t>Bud Śmietank Dr Oetk 40g</t>
+          <t>bud smietank dr oetk</t>
         </is>
       </c>
       <c r="M165" t="n">
@@ -9787,7 +9787,7 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>Szynka Od Szwagra Kg</t>
+          <t>szynka od szwagra kg</t>
         </is>
       </c>
       <c r="M166" t="inlineStr"/>
@@ -9837,7 +9837,7 @@
       <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr">
         <is>
-          <t>Kon Miel Lu Krak 300 g</t>
+          <t>kon miel lu krak</t>
         </is>
       </c>
       <c r="M167" t="n">
@@ -9845,7 +9845,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O167" t="n">
@@ -9901,7 +9901,7 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>Bocz. Węd/ Par 100g.</t>
+          <t xml:space="preserve">bocz wed par </t>
         </is>
       </c>
       <c r="M168" t="n">
@@ -9957,7 +9957,7 @@
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr">
         <is>
-          <t>Bud Waniliow Dr Oetk 40g</t>
+          <t>bud waniliow dr oetk</t>
         </is>
       </c>
       <c r="M169" t="n">
@@ -10013,7 +10013,7 @@
       <c r="K170" t="inlineStr"/>
       <c r="L170" t="inlineStr">
         <is>
-          <t>Kieł Kruchaz Gal kg</t>
+          <t>kiel kruchaz gal kg</t>
         </is>
       </c>
       <c r="M170" t="inlineStr"/>
@@ -10071,7 +10071,7 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>Jog nat Activ 165g</t>
+          <t>jog nat activ</t>
         </is>
       </c>
       <c r="M171" t="n">
@@ -10127,7 +10127,7 @@
       <c r="K172" t="inlineStr"/>
       <c r="L172" t="inlineStr">
         <is>
-          <t>Śmiet Pi 18 200g</t>
+          <t>smiet pi 18</t>
         </is>
       </c>
       <c r="M172" t="n">
@@ -10191,7 +10191,7 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>Pomarańcze Des Luz</t>
+          <t>pomarancze des luz</t>
         </is>
       </c>
       <c r="M173" t="inlineStr"/>
@@ -10241,7 +10241,7 @@
       <c r="K174" t="inlineStr"/>
       <c r="L174" t="inlineStr">
         <is>
-          <t>Papryka Słodka Żółta</t>
+          <t>papryka slodka zolta</t>
         </is>
       </c>
       <c r="M174" t="inlineStr"/>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>Pomid gał luz</t>
+          <t>pomid gal luz</t>
         </is>
       </c>
       <c r="M175" t="inlineStr"/>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>Pom Paprycz Luz</t>
+          <t>pom paprycz luz</t>
         </is>
       </c>
       <c r="M176" t="inlineStr"/>
@@ -10407,7 +10407,7 @@
       <c r="K177" t="inlineStr"/>
       <c r="L177" t="inlineStr">
         <is>
-          <t>Bat Energ Max AA 4szt</t>
+          <t>bat energ max aa</t>
         </is>
       </c>
       <c r="M177" t="n">
@@ -10463,7 +10463,7 @@
       <c r="K178" t="inlineStr"/>
       <c r="L178" t="inlineStr">
         <is>
-          <t>Masło Oseł Ml Dol 300g</t>
+          <t>maslo osel ml dol</t>
         </is>
       </c>
       <c r="M178" t="n">
@@ -10519,7 +10519,7 @@
       <c r="K179" t="inlineStr"/>
       <c r="L179" t="inlineStr">
         <is>
-          <t>Rol ZSer. Delik 100g</t>
+          <t>rol zser delik</t>
         </is>
       </c>
       <c r="M179" t="n">
@@ -10575,7 +10575,7 @@
       <c r="K180" t="inlineStr"/>
       <c r="L180" t="inlineStr">
         <is>
-          <t>Twaróg Półtł 250g</t>
+          <t>twarog poltl</t>
         </is>
       </c>
       <c r="M180" t="n">
@@ -10631,7 +10631,7 @@
       <c r="K181" t="inlineStr"/>
       <c r="L181" t="inlineStr">
         <is>
-          <t>Gru Kon Luz</t>
+          <t>gru kon luz</t>
         </is>
       </c>
       <c r="M181" t="inlineStr"/>
@@ -10689,7 +10689,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>Borówka Ameryk 300g</t>
+          <t>borowka ameryk</t>
         </is>
       </c>
       <c r="M182" t="n">
@@ -10745,7 +10745,7 @@
       <c r="K183" t="inlineStr"/>
       <c r="L183" t="inlineStr">
         <is>
-          <t>Pasztet Boro Gzel kg</t>
+          <t>pasztet boro gzel kg</t>
         </is>
       </c>
       <c r="M183" t="inlineStr"/>
@@ -10795,7 +10795,7 @@
       <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M184" t="n">
@@ -10851,7 +10851,7 @@
       <c r="K185" t="inlineStr"/>
       <c r="L185" t="inlineStr">
         <is>
-          <t>Kefir Krasnyst 420g</t>
+          <t>kefir krasnyst</t>
         </is>
       </c>
       <c r="M185" t="n">
@@ -10907,7 +10907,7 @@
       <c r="K186" t="inlineStr"/>
       <c r="L186" t="inlineStr">
         <is>
-          <t>Jaja Wol Wyb M 20szt</t>
+          <t>jaja wol wyb m</t>
         </is>
       </c>
       <c r="M186" t="n">
@@ -10963,7 +10963,7 @@
       <c r="K187" t="inlineStr"/>
       <c r="L187" t="inlineStr">
         <is>
-          <t>Fasol Heinz 415g</t>
+          <t>fasol heinz</t>
         </is>
       </c>
       <c r="M187" t="n">
@@ -11019,7 +11019,7 @@
       <c r="K188" t="inlineStr"/>
       <c r="L188" t="inlineStr">
         <is>
-          <t>Brokuły Mrożone MK 450g</t>
+          <t>brokuly mrozone mk</t>
         </is>
       </c>
       <c r="M188" t="n">
@@ -11075,7 +11075,7 @@
       <c r="K189" t="inlineStr"/>
       <c r="L189" t="inlineStr">
         <is>
-          <t>Mięs Miel Woł 400g</t>
+          <t>mies miel wol</t>
         </is>
       </c>
       <c r="M189" t="n">
@@ -11131,7 +11131,7 @@
       <c r="K190" t="inlineStr"/>
       <c r="L190" t="inlineStr">
         <is>
-          <t>Pierogi Ruskie 800g</t>
+          <t>pierogi ruskie</t>
         </is>
       </c>
       <c r="M190" t="n">
@@ -11187,7 +11187,7 @@
       <c r="K191" t="inlineStr"/>
       <c r="L191" t="inlineStr">
         <is>
-          <t>Ser Cheddar Wiór 300g</t>
+          <t>ser cheddar wior</t>
         </is>
       </c>
       <c r="M191" t="n">
@@ -11243,7 +11243,7 @@
       <c r="K192" t="inlineStr"/>
       <c r="L192" t="inlineStr">
         <is>
-          <t>Kieł śląs/biał 270g</t>
+          <t>kiel slasbial</t>
         </is>
       </c>
       <c r="M192" t="n">
@@ -11299,7 +11299,7 @@
       <c r="K193" t="inlineStr"/>
       <c r="L193" t="inlineStr">
         <is>
-          <t>ŚM PRIM 30 ZOT 200G</t>
+          <t>sm prim 30 zot</t>
         </is>
       </c>
       <c r="M193" t="n">
@@ -11355,7 +11355,7 @@
       <c r="K194" t="inlineStr"/>
       <c r="L194" t="inlineStr">
         <is>
-          <t>Serek Prot Wanilia 200g</t>
+          <t>serek prot wanilia</t>
         </is>
       </c>
       <c r="M194" t="n">
@@ -11419,7 +11419,7 @@
       </c>
       <c r="L195" t="inlineStr">
         <is>
-          <t>Bocz Słup Morl 130g</t>
+          <t>bocz slup morl</t>
         </is>
       </c>
       <c r="M195" t="n">
@@ -11475,7 +11475,7 @@
       <c r="K196" t="inlineStr"/>
       <c r="L196" t="inlineStr">
         <is>
-          <t>Pance Cube GB 150 g</t>
+          <t>pance cube gb</t>
         </is>
       </c>
       <c r="M196" t="n">
@@ -11483,7 +11483,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t xml:space="preserve"> g</t>
+          <t>g</t>
         </is>
       </c>
       <c r="O196" t="n">
@@ -11531,7 +11531,7 @@
       <c r="K197" t="inlineStr"/>
       <c r="L197" t="inlineStr">
         <is>
-          <t>Mięta Kolendra XLVF</t>
+          <t>mieta kolendra xlvf</t>
         </is>
       </c>
       <c r="M197" t="inlineStr"/>
@@ -11589,7 +11589,7 @@
       </c>
       <c r="L198" t="inlineStr">
         <is>
-          <t>Antipasti Peppe 150g</t>
+          <t>antipasti peppe</t>
         </is>
       </c>
       <c r="M198" t="n">
@@ -11653,7 +11653,7 @@
       </c>
       <c r="L199" t="inlineStr">
         <is>
-          <t>Ser Brie Intense 200g</t>
+          <t>ser brie intense</t>
         </is>
       </c>
       <c r="M199" t="n">
@@ -11709,7 +11709,7 @@
       <c r="K200" t="inlineStr"/>
       <c r="L200" t="inlineStr">
         <is>
-          <t>Cebula 1kg opak</t>
+          <t>cebula  opak</t>
         </is>
       </c>
       <c r="M200" t="n">
@@ -11765,7 +11765,7 @@
       <c r="K201" t="inlineStr"/>
       <c r="L201" t="inlineStr">
         <is>
-          <t>Banan Premium Luz</t>
+          <t>banan premium luz</t>
         </is>
       </c>
       <c r="M201" t="inlineStr"/>
@@ -11823,7 +11823,7 @@
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>Piwo Zatecky 0 0,5l</t>
+          <t>piwo zatecky 0</t>
         </is>
       </c>
       <c r="M202" t="n">
@@ -11879,7 +11879,7 @@
       <c r="K203" t="inlineStr"/>
       <c r="L203" t="inlineStr">
         <is>
-          <t>Chipsy Kett Sól Vin 150g</t>
+          <t>chipsy kett sol vin</t>
         </is>
       </c>
       <c r="M203" t="n">
@@ -11935,7 +11935,7 @@
       <c r="K204" t="inlineStr"/>
       <c r="L204" t="inlineStr">
         <is>
-          <t>P Oko Rad Ci Wiśn 0,5l</t>
+          <t>p oko rad ci wisn</t>
         </is>
       </c>
       <c r="M204" t="n">
@@ -11991,7 +11991,7 @@
       <c r="K205" t="inlineStr"/>
       <c r="L205" t="inlineStr">
         <is>
-          <t>Piwo Żyw Malin 0 0,5L</t>
+          <t>piwo zyw malin 0</t>
         </is>
       </c>
       <c r="M205" t="n">
@@ -12047,7 +12047,7 @@
       <c r="K206" t="inlineStr"/>
       <c r="L206" t="inlineStr">
         <is>
-          <t>Des. La Speci 100g</t>
+          <t>des la speci</t>
         </is>
       </c>
       <c r="M206" t="n">
@@ -12103,7 +12103,7 @@
       <c r="K207" t="inlineStr"/>
       <c r="L207" t="inlineStr">
         <is>
-          <t>Pizza Prosc GB 430g</t>
+          <t>pizza prosc gb</t>
         </is>
       </c>
       <c r="M207" t="n">
@@ -12167,7 +12167,7 @@
       </c>
       <c r="L208" t="inlineStr">
         <is>
-          <t>Deser Monte 150g</t>
+          <t>deser monte</t>
         </is>
       </c>
       <c r="M208" t="n">
@@ -12231,7 +12231,7 @@
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>Woda NGaz Muszy 1,5l</t>
+          <t>woda ngaz muszy</t>
         </is>
       </c>
       <c r="M209" t="n">
@@ -12247,6 +12247,856 @@
       </c>
       <c r="P209" t="n">
         <v>13.14</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>FasolHeinz 415g          C</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>729</v>
+      </c>
+      <c r="F210" t="n">
+        <v>2187</v>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr"/>
+      <c r="I210" t="inlineStr"/>
+      <c r="J210" t="inlineStr"/>
+      <c r="K210" t="inlineStr"/>
+      <c r="L210" t="inlineStr">
+        <is>
+          <t>fasol heinz</t>
+        </is>
+      </c>
+      <c r="M210" t="n">
+        <v>415</v>
+      </c>
+      <c r="N210" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O210" t="n">
+        <v>2187</v>
+      </c>
+      <c r="P210" t="n">
+        <v>21.87</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>SerekProt.Malina200g     C</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>335</v>
+      </c>
+      <c r="F211" t="n">
+        <v>335</v>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr"/>
+      <c r="I211" t="inlineStr"/>
+      <c r="J211" t="inlineStr"/>
+      <c r="K211" t="inlineStr"/>
+      <c r="L211" t="inlineStr">
+        <is>
+          <t>serek prot malina</t>
+        </is>
+      </c>
+      <c r="M211" t="n">
+        <v>200</v>
+      </c>
+      <c r="N211" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O211" t="n">
+        <v>335</v>
+      </c>
+      <c r="P211" t="n">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>SerekProtWanilia200g     C</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>335</v>
+      </c>
+      <c r="F212" t="n">
+        <v>335</v>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr"/>
+      <c r="I212" t="inlineStr"/>
+      <c r="J212" t="inlineStr"/>
+      <c r="K212" t="inlineStr"/>
+      <c r="L212" t="inlineStr">
+        <is>
+          <t>serek prot wanilia</t>
+        </is>
+      </c>
+      <c r="M212" t="n">
+        <v>200</v>
+      </c>
+      <c r="N212" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O212" t="n">
+        <v>335</v>
+      </c>
+      <c r="P212" t="n">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>JajaWolWybM20szt         C</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>2045</v>
+      </c>
+      <c r="F213" t="n">
+        <v>2045</v>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr"/>
+      <c r="I213" t="inlineStr"/>
+      <c r="J213" t="inlineStr"/>
+      <c r="K213" t="inlineStr"/>
+      <c r="L213" t="inlineStr">
+        <is>
+          <t>jaja wol wyb m</t>
+        </is>
+      </c>
+      <c r="M213" t="n">
+        <v>20</v>
+      </c>
+      <c r="N213" t="inlineStr">
+        <is>
+          <t>szt</t>
+        </is>
+      </c>
+      <c r="O213" t="n">
+        <v>2045</v>
+      </c>
+      <c r="P213" t="n">
+        <v>20.45</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Miesz Chińska 450g       C</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>399</v>
+      </c>
+      <c r="F214" t="n">
+        <v>1596</v>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr"/>
+      <c r="I214" t="inlineStr"/>
+      <c r="J214" t="inlineStr"/>
+      <c r="K214" t="inlineStr"/>
+      <c r="L214" t="inlineStr">
+        <is>
+          <t>miesz chinska</t>
+        </is>
+      </c>
+      <c r="M214" t="n">
+        <v>450</v>
+      </c>
+      <c r="N214" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O214" t="n">
+        <v>1596</v>
+      </c>
+      <c r="P214" t="n">
+        <v>15.96</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>BrokułyMrożoneMK450g     C</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>549</v>
+      </c>
+      <c r="F215" t="n">
+        <v>549</v>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr"/>
+      <c r="I215" t="inlineStr"/>
+      <c r="J215" t="inlineStr"/>
+      <c r="K215" t="inlineStr"/>
+      <c r="L215" t="inlineStr">
+        <is>
+          <t>brokuly mrozone mk</t>
+        </is>
+      </c>
+      <c r="M215" t="n">
+        <v>450</v>
+      </c>
+      <c r="N215" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O215" t="n">
+        <v>549</v>
+      </c>
+      <c r="P215" t="n">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>MłPieprCzKamis42 g       B</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>899</v>
+      </c>
+      <c r="F216" t="n">
+        <v>899</v>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr"/>
+      <c r="I216" t="inlineStr"/>
+      <c r="J216" t="inlineStr"/>
+      <c r="K216" t="inlineStr"/>
+      <c r="L216" t="inlineStr">
+        <is>
+          <t>ml piepr cz kamis</t>
+        </is>
+      </c>
+      <c r="M216" t="n">
+        <v>42</v>
+      </c>
+      <c r="N216" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O216" t="n">
+        <v>899</v>
+      </c>
+      <c r="P216" t="n">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>MłynSólMorKami90 g       A</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>899</v>
+      </c>
+      <c r="F217" t="n">
+        <v>899</v>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr"/>
+      <c r="I217" t="inlineStr"/>
+      <c r="J217" t="inlineStr"/>
+      <c r="K217" t="inlineStr"/>
+      <c r="L217" t="inlineStr">
+        <is>
+          <t>mlyn sol mor kami</t>
+        </is>
+      </c>
+      <c r="M217" t="n">
+        <v>90</v>
+      </c>
+      <c r="N217" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O217" t="n">
+        <v>899</v>
+      </c>
+      <c r="P217" t="n">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>KawRozCrGoldJa200g       A</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>3199</v>
+      </c>
+      <c r="F218" t="n">
+        <v>6398</v>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H218" t="n">
+        <v>6398</v>
+      </c>
+      <c r="I218" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J218" t="b">
+        <v>1</v>
+      </c>
+      <c r="K218" t="b">
+        <v>0</v>
+      </c>
+      <c r="L218" t="inlineStr">
+        <is>
+          <t>kaw roz cr gold ja</t>
+        </is>
+      </c>
+      <c r="M218" t="n">
+        <v>200</v>
+      </c>
+      <c r="N218" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O218" t="n">
+        <v>4798</v>
+      </c>
+      <c r="P218" t="n">
+        <v>47.98</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>PaluszkiLajkon200g       C</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>469</v>
+      </c>
+      <c r="F219" t="n">
+        <v>469</v>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr"/>
+      <c r="I219" t="inlineStr"/>
+      <c r="J219" t="inlineStr"/>
+      <c r="K219" t="inlineStr"/>
+      <c r="L219" t="inlineStr">
+        <is>
+          <t>paluszki lajkon</t>
+        </is>
+      </c>
+      <c r="M219" t="n">
+        <v>200</v>
+      </c>
+      <c r="N219" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O219" t="n">
+        <v>469</v>
+      </c>
+      <c r="P219" t="n">
+        <v>4.69</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>ŚledzieTapasMix130g      C</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>599</v>
+      </c>
+      <c r="F220" t="n">
+        <v>599</v>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H220" t="n">
+        <v>599</v>
+      </c>
+      <c r="I220" t="n">
+        <v>300</v>
+      </c>
+      <c r="J220" t="b">
+        <v>1</v>
+      </c>
+      <c r="K220" t="b">
+        <v>0</v>
+      </c>
+      <c r="L220" t="inlineStr">
+        <is>
+          <t>sledzie tapas mix</t>
+        </is>
+      </c>
+      <c r="M220" t="n">
+        <v>130</v>
+      </c>
+      <c r="N220" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O220" t="n">
+        <v>299</v>
+      </c>
+      <c r="P220" t="n">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Kieł.śląs/biał270g       C</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>999</v>
+      </c>
+      <c r="F221" t="n">
+        <v>1998</v>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr"/>
+      <c r="I221" t="inlineStr"/>
+      <c r="J221" t="inlineStr"/>
+      <c r="K221" t="inlineStr"/>
+      <c r="L221" t="inlineStr">
+        <is>
+          <t>kiel slasbial</t>
+        </is>
+      </c>
+      <c r="M221" t="n">
+        <v>270</v>
+      </c>
+      <c r="N221" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O221" t="n">
+        <v>1998</v>
+      </c>
+      <c r="P221" t="n">
+        <v>19.98</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>MmilcProtZeroCze400g     C</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>529</v>
+      </c>
+      <c r="F222" t="n">
+        <v>1058</v>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr"/>
+      <c r="I222" t="inlineStr"/>
+      <c r="J222" t="inlineStr"/>
+      <c r="K222" t="inlineStr"/>
+      <c r="L222" t="inlineStr">
+        <is>
+          <t>mmilc prot zero cze</t>
+        </is>
+      </c>
+      <c r="M222" t="n">
+        <v>400</v>
+      </c>
+      <c r="N222" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O222" t="n">
+        <v>1058</v>
+      </c>
+      <c r="P222" t="n">
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>PuddingCzekDesel180g     C</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>155</v>
+      </c>
+      <c r="F223" t="n">
+        <v>155</v>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr"/>
+      <c r="I223" t="inlineStr"/>
+      <c r="J223" t="inlineStr"/>
+      <c r="K223" t="inlineStr"/>
+      <c r="L223" t="inlineStr">
+        <is>
+          <t>pudding czek desel</t>
+        </is>
+      </c>
+      <c r="M223" t="n">
+        <v>180</v>
+      </c>
+      <c r="N223" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="O223" t="n">
+        <v>155</v>
+      </c>
+      <c r="P223" t="n">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>15:21:48</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>PietruszkaDonXLVF        C</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>799</v>
+      </c>
+      <c r="F224" t="n">
+        <v>799</v>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr"/>
+      <c r="I224" t="inlineStr"/>
+      <c r="J224" t="inlineStr"/>
+      <c r="K224" t="inlineStr"/>
+      <c r="L224" t="inlineStr">
+        <is>
+          <t>pietruszka don xlvf</t>
+        </is>
+      </c>
+      <c r="M224" t="inlineStr"/>
+      <c r="N224" t="inlineStr"/>
+      <c r="O224" t="n">
+        <v>799</v>
+      </c>
+      <c r="P224" t="n">
+        <v>7.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>